<commit_message>
Created files to track spread cover
</commit_message>
<xml_diff>
--- a/WNBA_Basketball_6.7.2022.xlsx
+++ b/WNBA_Basketball_6.7.2022.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahtaylor/Desktop/Personal Data Projects/SportsBettingOdds/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C916C7B6-FCE8-8343-9B9F-5E8CC70EF557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Best Sports Book(HT)</t>
   </si>
@@ -53,13 +59,28 @@
   </si>
   <si>
     <t>Atlanta Dream</t>
+  </si>
+  <si>
+    <t>Favored Team Final Score</t>
+  </si>
+  <si>
+    <t>Underdog Team Final Score</t>
+  </si>
+  <si>
+    <t>Home Team Cover</t>
+  </si>
+  <si>
+    <t>Favored Team Cover?</t>
+  </si>
+  <si>
+    <t>Underdog Team Cover?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +105,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,13 +128,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -122,6 +157,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -168,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -200,9 +243,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,6 +295,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -409,14 +488,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -438,8 +532,23 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -462,7 +571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>

</xml_diff>